<commit_message>
part 2 - WIP
</commit_message>
<xml_diff>
--- a/Convert input to array.xlsx
+++ b/Convert input to array.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardbrain/Dropbox/Dev Career/Advent of Code/Day_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7226C72-58C7-474A-AFC0-C8B2E391D94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234C5435-205A-824E-B866-6700BAEBC205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8000" yWindow="4560" windowWidth="28040" windowHeight="17440" xr2:uid="{2A895845-F684-0A40-96F0-D33697391A64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2981,8 +2981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65132035-2F8E-2840-BE1E-72F9DAE642FB}">
   <dimension ref="A1:G4104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1135" workbookViewId="0">
-      <selection activeCell="G1140" sqref="G1140"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3005,8 +3005,8 @@
         <v>"R19",</v>
       </c>
       <c r="G2" t="str">
-        <f>_xlfn.CONCAT("const listOfInputs = ",CHAR(91),D1:D4104,CHAR(92),";")</f>
-        <v>const listOfInputs = ["R9","R19","R34","R38","L47","R30","R36","L35","L25","L10","L6","R38","R16","R43","L37","R48","R23","L19","R22","L17","R1","R13","R26","R11","R31","R42","L22","R41","R21","R3","R24","L22","L28","L6","L21","L37","L17","L25","R43","L21","L4","L28","R16","L49","R46","R37","R14","R42","L12","L29","L36","L64","R67","L12","L96","L93","R38","R96","R70","L43","L27","R29","R43","L95","L72","L5","L73","R73","L3","R83","L88","L69","R86","R20","L97","R70","L77","R75","R40","L95","L10","R50","L85","R84","R16","R74","L74","R43","L85","L58","L95","R95","L44","R44","L68","L32","L97","L4","R50","R32","R19","L29","R829","R41","L15","L26","L83","L77","R60","L74","R34","L91","L22","R53","R898","L98","R49","R51","R99","R70","L69","L24","R24","R5","R95","L48","L38","R66","R61","R33","L74","R762","L750","R90","L802","L10","R190","L80","L85","L15","R738","L54","R16","R81","L90","R38","R76","R65","L76","R71","R35","L85","L54","L261","R868","L3","R663","R72","R22","R37","L59","R524","L12","L12","R69","L47","R974","R579","R84","R276","L35","R350","L50","L36","R36","R7","R11","R89","R87","R6","R23","R93","L16","L43","R33","R635","L16","L86","R52","L575","R74","R26","R10","R96","L6","R33","L505","R84","R98","L59","L831","L39","R21","L2","L606","L45","L90","L63","R47","R80","R985","R29","L237","R41","L3","L38","L44","R27","L83","L89","L65","R27","L86","R89","L32","R44","R212","L74","R97","R77","R91","R9","R83","R17","L55","R9","R46","R480","L63","R83","L71","L29","R252","L567","L97","R56","R56","L77","R22","R86","R8","L23","R84","R91","L44","R23","L70","L21","R21","R27","R12","R24","R37","L206","R360","L241","L12","L93","L48","L96","L95","L18","R23","L14","R46","R69","R25","R7","L68","L44","R5","L268","R68","R1","L1","R280","L980","L131","L192","R34","R36","L47","L37","L145","L948","R930","R14","R46","R40","L517","L24","L836","R37","L960","L49","L31","R535","L55","L11","R72","R56","R83","R25","L225","L70","L25","L48","L966","R709","L9","L91","R53","L5","R52","L14","R641","R73","L57","R960","R36","R26","R477","L85","R609","L66","L28","R54","L26","L41","L69","L6","L49","R18","L19","R45","R21","R44","L32","R88","L65","R6","R45","L75","R24","R133","R32","R81","L6","R29","L504","R77","L84","R58","L39","R57","L969","L55","L5","L864","R81","L43","L14","R10","L128","L85","R3","R9","L9","R99","R207","L84","L90","R71","R278","R58","L39","L33","L67","L378","R58","R92","L6","R34","L89","L55","R94","L78","L77","R55","R650","L4","R67","L191","L772","L72","R84","R59","L97","R26","R98","R48","R16","R19","R13","L44","R50","R71","R29","R27","L14","R687","R79","R236","L396","R81","L27","L32","R659","L54","R67","L13","L92","R6","L17","R10","R426","R793","L14","L35","R28","L5","R53","L23","L21","L31","R822","L35","L579","R30","R37","R50","R194","R3","R53","L940","R309","R378","L91","R7","L52","R65","L26","R16","R237","R68","L581","L26","R83","L92","L45","R176","R49","L45","R18","R481","R68","R44","L63","L291","R67","L554","L721","L7","R15","L53","R53","R69","R14","R94","R35","R12","L24","L90","L36","L66","L939","R31","L70","R970","R562","R85","L23","R95","R81","L19","L33","L48","R53","L129","R76","R216","L91","R95","L20","R69","L65","R96","R72","R28","R17","L11","L96","R170","L87","R33","L83","R657","R65","R58","R72","R5","R49","L38","L34","L477","R87","L69","L75","L913","R995","L25","R66","L19","R258","L537","R13","R19","R53","L53","R74","L74","R938","R95","L33","R72","R28","L64","R25","L56","L272","R73","R68","L41","R22","R6","L961","L825","R325","R67","R95","R38","R41","L68","R27","L75","R75","L97","R60","L62","R90","L73","L393","R25","L50","L375","L67","L58","L92","L608","R13","L295","L18","R63","L95","R32","L952","L18","R799","L80","L48","L1","R10","R90","L824","R91","L67","L24","R33","R16","L25","R76","R24","R63","L40","R1","R66","L90","L74","R374","L87","R942","R945","L83","R64","L89","R32","L577","R9","R13","L59","L87","L21","L356","L46","R421","R79","R55","L42","R87","L53","L47","L66","L49","R15","R81","R73","R822","R923","L454","R44","L89","R23","L592","R69","L18","R17","R65","L89","R55","L30","R61","R53","R82","R97","R605","R2","L3","R814","R1","R64","L76","R39","R21","R40","R105","R23","R72","R54","R533","R28","L15","L49","R49","L92","L2","L206","L69","R82","L913","L89","L11","L25","L151","R76","L43","R97","L54","R859","L274","L322","L134","L29","L83","R583","L685","R366","L7","L10","R36","R33","R35","L43","R82","L7","R593","R492","L85","L927","R4","L53","L24","R29","R222","L922","L594","R41","L76","R251","L47","L57","L91","L56","R24","L22","L70","R31","R525","L32","L796","R56","R7","R677","R29","R88","R65","R18","R19","L23","R904","L23","R41","L318","R65","R42","L99","L63","R15","L78","L57","L33","L84","R34","R87","R624","L30","L97","R24","R35","R67","R48","L59","L35","L70","L97","L69","L55","L550","L82","L89","R78","R828","L44","R286","R558","R42","L13","R53","R58","R63","R808","R999","L457","R47","R94","R65","L88","R30","L48","L75","R523","R32","R70","L3","R93","R59","L52","R51","R2","R897","L914","L36","L47","L861","R65","R91","R38","R32","R282","R10","R16","R70","L16","L38","R58","L21","R81","L78","R18","L422","R22","L304","L96","L54","R61","R32","L39","R371","L71","L89","L8","L403","L688","L21","L388","R16","R807","R82","R161","R96","R635","R426","R38","L59","R58","L17","R619","L59","L93","L13","L384","L16","L5","L636","L68","L91","R66","L66","R31","L63","L57","L56","L55","R853","R464","L92","R475","L640","R40","L16","L484","R87","R87","L394","L80","R64","L42","R12","L39","L31","L25","L49","R48","R62","L90","R90","L78","R13","R89","R74","R77","L549","L4","L22","R89","R54","L8","L35","L61","R27","R41","R7","R86","L27","L73","L42","R88","R818","L15","R58","L48","L5","R780","L24","L1","L9","L3","L97","R64","L9","R16","L71","R893","L87","R427","R55","R5","L93","L36","R1","L89","L60","R91","L7","R83","L51","L55","R23","L7","R7","L65","R65","R1","L24","L35","R658","L51","L149","R88","R1","L89","R74","L74","L644","R218","L52","R78","R21","L21","L296","R96","R909","L38","R343","L45","L62","L702","R77","L682","L21","R21","R72","R428","L61","L39","R61","R39","R94","L51","R22","R725","R482","R28","L84","R84","L56","R56","R502","R24","L364","L865","R403","R25","R575","L74","L89","R863","R51","L220","L31","R8","L73","L35","L29","R199","R96","R72","L76","L60","R67","L43","R74","R955","R79","R17","L12","L2","L20","R29","R95","L46","R589","R16","R11","L151","R76","L36","R737","R63","R19","L69","R50","L53","R242","L47","L96","R69","L15","L72","R65","R939","L92","L56","L84","R76","R24","R92","L59","L454","R36","R82","L97","R66","L394","R14","L76","R20","R28","R47","L5","L581","L19","R67","R11","R46","R69","L93","L1","L4","L95","L50","R85","R382","L98","L8","R9","L20","R92","R8","R2","L6","R704","R98","L86","R60","R99","R66","R63","L867","L333","R21","R67","L74","L14","R7","L12","R52","L17","L130","L659","R505","R79","R75","L69","L81","R50","L6","L40","R46","L72","R57","R41","R74","R25","R510","L35","R18","L436","L713","L91","L4","L374","L5","L95","R12","R88","L92","L19","R9","L98","R98","R984","R18","R68","R32","R61","L26","L76","R36","L65","R70","L339","R39","L89","R30","R30","L115","L56","R705","L18","L936","R64","R85","L74","L795","L31","R57","R46","L425","R92","L70","R71","L98","R727","R12","R479","R109","R1","L4","R60","R43","R815","R316","L440","R11","L55","L88","R97","L70","L38","R50","R2","R24","R76","L19","L81","R537","R63","L16","L35","R690","L2","L6","L31","R44","L49","R905","R44","R32","L473","L8","R39","R67","R78","L18","R334","L92","R97","L8","L13","R18","L97","R226","R74","R94","R179","R67","R860","L247","L72","R21","R98","R59","R9","L78","L525","L65","R89","L16","R27","R55","L198","L53","R96","R31","L731","L29","R29","L9","R35","R62","R530","R404","R78","R15","L815","L799","L201","L92","R98","L506","R31","L27","R302","L50","L69","L34","R97","L363","L58","R97","L59","R91","R42","L16","R16","R839","R61","L828","R26","L49","L49","R87","R813","L63","R891","R372","L94","R253","R39","L367","R869","L73","L33","R72","L166","L201","R96","R38","R58","L91","L45","L36","L719","R12","L89","L38","R15","R313","L77","L36","L41","R48","R50","R543","R78","R98","L12","R24","L665","R4","L27","R30","R414","R6","L12","R97","R22","L870","R62","L49","L26","L31","L43","L66","R231","L19","R46","R30","L22","R13","R57","L151","L819","L88","R64","L76","R40","L840","R59","L64","L46","L81","L926","R579","L68","L270","L83","L55","R55","R774","L74","R92","L5","R75","R54","R84","R77","L277","L703","L97","L3","R96","L93","R29","R3","R60","L32","L68","L592","R98","R2","R6","L871","L22","L53","L49","L611","L89","L32","R47","L319","L42","L65","R68","L68","L21","R21","L695","L5","L770","R95","R75","R6","L85","R79","L28","L72","R98","R48","R945","L15","L52","L44","L32","R980","R72","L6","L408","L79","R693","L32","L13","L12","L18","R94","R81","R162","R638","R738","L38","R91","L29","R46","R167","L9","L355","L96","L27","L59","L29","R23","R77","L36","R57","L21","L69","L31","L940","L960","L36","R67","R35","R29","R5","R24","R78","R98","L26","R69","L47","R4","L41","R41","L83","L74","R80","R21","R56","R684","R51","L35","R863","L23","R61","L801","L47","R51","R80","R81","L7","R442","R27","R73","R73","R87","L963","L97","R14","L14","L24","R15","L291","R33","R97","L263","R11","R12","R10","R445","L12","L45","R612","L519","L81","R53","L53","L65","R565","R34","R66","L93","R16","R58","R25","L81","L17","R92","R55","R56","R40","L15","R67","R97","R93","R7","L69","R59","L42","R24","R74","R654","R24","L24","R35","R65","R34","R81","L4","R8","L59","R53","R57","L70","L33","R90","R92","L49","R54","R51","L119","L11","L75","R56","L528","R572","L14","L86","L9","R9","L73","R84","L311","R86","L86","L60","L40","R45","R155","L74","R93","R595","R83","L301","L90","L52","L1","L74","R99","R297","R32","L753","R46","R29","R299","L306","L22","L75","R62","L87","R88","L14","L246","R21","L14","L55","L80","R86","L33","L53","R508","R592","L6","L15","R6","L47","L95","R29","L72","L332","R432","L446","L58","L96","L40","R66","R17","R457","R57","R75","L950","R32","R95","L9","L55","R206","R23","L96","L78","R27","L115","L12","R3","R18","R79","L33","L62","R53","L6","L52","R60","R40","L27","R97","R27","R3","R495","R207","L2","L10","R73","L63","R94","L39","R92","L75","R28","R82","R18","R978","R22","L8","L92","L61","L909","R102","L32","R40","R19","L40","L419","L7","R7","L25","R25","R53","R247","L37","L763","L56","R604","R296","R56","R40","R94","R694","L13","L88","R203","L66","R33","L41","R44","L679","L531","L2","R3","R22","L74","L47","L31","R54","R85","L564","L930","L642","L81","L69","L79","L20","R485","L503","L42","R293","L93","L55","R13","L13","L8","R896","L34","R272","L26","R73","L762","L11","R90","R510","L313","R51","R228","L66","L23","R28","R94","L899","R38","L38","L77","L589","L50","R16","L88","R42","L82","L72","L28","R528","R47","L93","L54","R14","L14","L49","L51","L50","L63","R54","L41","L86","R43","R81","R88","L79","L47","L24","L76","R93","R891","R21","R95","L56","L37","R689","R53","R51","R26","R161","R30","R83","R82","R98","R17","R98","R805","R68","L92","L4","R28","L418","R95","R53","L33","L497","L13","L282","R43","L69","L59","R80","L37","L55","L32","L40","L87","R421","R67","R963","L77","R77","L323","R147","R239","R7","R30","L35","R985","R50","R10","L921","L89","R23","L188","L73","R10","L72","L83","R18","L7","R72","R5","L5","L56","R51","L20","L75","L43","R26","L82","R83","L872","L551","R7","L68","L94","R44","R56","R4","L10","R82","R30","L44","L603","R685","L98","L70","R9","L47","R36","R587","R80","R55","L302","L96","L47","R54","L11","L92","L8","L61","R61","R71","R58","L29","L24","L6","L22","R98","R660","R94","L15","R515","L211","R11","R42","R45","R813","L66","L50","R30","L114","R60","R57","L96","L21","L641","L59","L49","R425","L76","R18","R82","L69","L26","L980","L40","L85","R75","L90","R15","R50","L55","L95","R891","L891","R311","R741","R9","R639","L581","R81","R29","R71","L12","L94","R16","L10","L82","L70","R36","L84","R553","L53","L10","L90","R730","R32","R38","L26","R26","L418","R65","R47","R6","L40","L60","L7","R307","R84","R416","R26","R92","L22","R42","L62","L76","L380","L66","L54","L772","R72","R62","L33","R71","L12","L64","L24","L56","L95","L8","R59","R90","L90","L83","R38","L55","L889","L77","R466","R76","L790","L44","R58","R31","L71","R40","R74","L74","R5","L19","R214","R16","L16","R6","L65","R59","L56","R7","L357","L77","L47","R734","L15","L39","R66","R55","R371","R48","L684","L6","L71","L929","R82","L83","R1","L33","R61","L13","R30","L52","L93","L61","L39","R61","L61","L94","L509","R94","R95","R14","L45","L55","R72","L22","R650","L661","R61","L64","L36","L87","R887","L83","R12","R82","R646","R84","L57","L55","L97","R90","L32","L90","R476","R31","R93","R320","R80","R24","L78","L46","L90","R3","R22","R33","L31","L694","R22","R335","R86","R314","R66","L458","R92","R363","R50","L99","L13","R6","L7","R690","R706","R22","L99","R69","L88","R19","L3","L16","L377","L64","L57","L3","L90","R53","R38","L21","R44","R77","R3","L29","L74","R34","R98","L932","R10","R81","R760","R77","L927","R99","L42","R73","R95","R899","R75","L41","L17","R78","R70","L90","R53","L37","R25","L86","R13","L72","R61","R759","L14","L78","R24","R252","R17","L17","L89","L49","L62","R222","R21","L43","R2","R41","R49","R42","L81","R67","R4","L27","R60","L57","L305","L11","L84","L72","L352","R256","L838","R19","L51","L62","L35","L65","L92","L58","R689","R61","R201","R399","L63","R83","L97","R77","R575","L75","L73","L72","L395","R26","R629","L61","L35","L44","R825","L34","R34","L56","R68","R88","R92","R608","L260","R89","L829","R74","R17","L91","L26","L564","L10","L98","L802","R12","L12","R33","L933","L58","R67","R17","L26","R83","R92","R25","L399","L1","L16","R61","R108","R47","L621","L73","R24","L848","L71","L454","R543","L213","L40","L62","R15","L86","L77","L37","R37","L637","R63","L75","R12","R23","R77","R9","R23","L743","L89","R948","L902","R54","R66","L352","L17","R3","L43","L80","L78","R201","L4","L58","L438","R39","L25","L67","L55","L294","R7","L93","L212","L71","R71","R781","R27","L72","R11","R45","L97","R240","L13","L56","L66","L90","R7","L17","L21","L38","L41","L36","L37","R473","L31","L32","L637","R19","L19","L49","L65","L86","L838","L7","L859","R55","R28","R21","L138","R438","R30","L30","L51","R324","R96","L69","L31","R79","L48","L95","L5","R121","R79","L324","R17","L93","L534","L7","L937","R97","R983","R3","L84","L21","R4","R533","L437","L1","R47","R16","L12","L265","R2","R13","L71","R71","L99","R81","R18","R821","R57","R22","L67","R89","L49","L73","R77","R680","R79","R10","R83","L29","L87","R248","L10","L23","R79","L367","R23","L463","L86","R97","L91","R69","L64","L757","R3","R29","R21","L201","R80","L58","L42","L230","L52","L35","R39","L4","L177","L26","L55","R740","L96","L261","L83","L99","R57","L18","L52","L76","L372","R45","L35","L59","R34","R375","L277","L96","R916","R96","L55","L146","L171","L127","R42","L42","L507","R33","R74","L88","R58","L20","R50","R31","L11","L20","L26","R694","R39","L39","R58","L998","R36","R89","R21","R76","L80","R32","L76","R80","L6","R54","L20","R56","L290","L90","L10","R21","L29","R8","L97","R23","R73","R23","L22","L54","L9","L55","R334","R91","L20","R113","R467","R833","L93","R544","R78","R61","L90","L75","L25","R695","L95","L70","R470","L92","L11","L97","L38","L11","R51","L91","L82","L29","R30","L844","L86","L22","R722","R99","R446","R55","L8","R525","R83","L13","R72","L92","R333","L33","L67","R439","R461","L790","L566","L97","R53","L66","R14","L9","L39","L60","R68","R91","L38","L61","L890","L910","R774","R826","L97","L33","L56","L5","L39","R930","L295","L59","R54","R3","R797","R71","R61","R28","R53","R26","R96","R82","L126","R66","R43","R70","R20","L421","L71","R70","L19","L52","L597","L97","R97","L85","L15","L70","R76","R94","R79","R13","L92","R51","R58","R49","R63","R16","R48","R15","L38","R26","R12","R62","L62","L24","R81","R43","R1","R899","R58","L753","L56","R18","R26","R1","R6","R33","R67","L58","L72","L770","R41","R46","R87","L437","L34","R63","R34","L60","L73","L2","L88","R23","L11","L75","L414","L84","R84","L40","L87","R327","L90","R53","L92","L71","L875","L44","L50","L5","R94","R32","L96","R13","L69","R28","L28","L58","R92","R94","R63","L568","L423","L22","R4","R67","L29","R69","R11","R7","L7","L5","L227","R32","L26","L74","L7","L921","L487","R15","R927","L95","R62","L93","R2","L3","R50","L50","L99","R99","L691","L134","L75","L76","R670","R53","L491","L352","L10","R6","R19","L79","R23","L837","R55","L23","L46","L12","L22","L76","L31","L286","R50","R65","L28","L54","R82","R88","R699","L158","L22","L89","R98","L199","R461","R22","R1","R899","L126","L74","L55","R555","R1","L31","R78","L39","R846","R45","R20","L71","R78","R27","R21","R925","R36","R71","R68","L375","L66","R489","L523","R29","L29","R6","L306","L889","L11","L73","L95","L307","R7","L11","L51","R630","L82","L5","L638","R25","R688","R4","R8","L89","L95","L21","R57","R48","R29","R914","L96","R53","L561","L39","R14","L14","R35","L351","R38","R576","L34","L964","L76","R176","L88","R83","R436","R471","R96","R7","R56","L95","R5","R82","R41","L57","L37","R476","L76","R46","L90","L93","R7","R81","R570","R79","L68","L86","R92","R32","R30","L648","L52","R65","R237","L94","R39","L947","L2","L998","R23","R64","L195","L92","R663","R66","R72","L97","L807","L978","R81","R21","L68","L895","R16","L1","L54","R99","L6","R77","R59","L83","R35","R45","L45","R4","L28","L4","R28","L753","R377","R76","L98","L931","L43","R28","R477","L33","L22","L378","L74","R74","R947","L505","L58","R16","L74","L982","L866","L37","R59","L774","R636","L3","R41","R523","L23","L84","L437","L79","L71","R71","L22","L74","L76","R72","R93","R7","R89","L89","R7","R11","R724","R68","R190","L54","L827","R245","L64","L79","L17","R938","R83","L35","R10","R52","R943","R73","R6","L68","L6","L56","L544","L39","L849","L867","R55","L715","L70","L48","L67","R96","R79","R25","R639","L39","L60","R55","L95","L88","L12","R62","R272","R85","R81","R67","L78","L56","L58","L201","R80","R46","R97","L95","R98","L1","R815","L14","L57","L95","R52","L22","R22","R19","R34","L78","R25","L20","L863","L17","L93","L97","R77","L44","R84","R17","R56","R1","R199","L91","L864","L188","R43","R95","R726","L73","R44","R8","L65","R65","R29","R786","L85","R70","L72","R577","R495","R96","R4","L51","R39","R12","L13","L42","L87","R46","L4","R63","R29","L57","L411","L745","L60","L1","L518","L75","L25","L910","L28","L62","L67","L65","L68","R19","R81","R74","L74","R41","L72","L769","L68","R68","L35","R35","R92","R88","R20","R76","L76","R78","L478","R28","R72","R69","L69","L10","R10","R806","R13","R81","L31","R57","L16","R289","L23","L62","L40","L74","L77","L28","R5","R544","R47","L57","L88","R47","R311","R9","L13","R55","L38","L17","L22","R22","L50","R750","R175","L93","L82","R9","R98","R73","L2","R22","L34","L37","R59","L88","R361","L1","R4","R36","L29","L42","R40","L93","L76","L82","L36","L17","L420","L50","R71","L94","L720","L441","R89","L726","R826","L741","L59","L46","L213","R464","R95","R98","L98","R135","L23","R21","R67","R56","L56","R54","R46","R33","L33","R45","R55","L635","R306","L2","R74","L678","R26","L99","R18","L10","L71","L29","R83","R213","L478","R19","R63","R796","L71","R59","R19","R48","L15","L17","L18","R26","L27","R9","R163","L507","R41","L6","R25","R579","L4","R949","R43","R8","R68","R22","R51","R35","R38","R388","R66","L68","R71","L71","R54","L54","R477","R14","R75","R32","R650","R30","L78","R34","L34","L65","L99","R44","L80","R339","L78","L23","L87","R37","R86","L474","R27","L94","L33","L75","L25","L57","R57","R26","R75","R352","R5","R42","L49","L69","R196","R61","R26","R43","R9","R14","L37","R11","L105","R41","R37","R8","L86","L85","L15","L154","L746","L571","R30","L59","L2","R11","L84","R66","R41","L32","R44","R56","R35","L26","R15","L43","L81","R32","R68","R22","R78","L976","R76","L776","L21","L3","R980","R76","L656","L42","L858","L288","R188","R15","R39","R67","R72","R98","L970","L28","L793","L56","R240","L86","R40","L77","L14","R14","R41","R95","L1","R4","L270","R70","L10","R48","R62","L99","L1","R626","L26","L33","R231","L63","R65","L47","R91","R6","L92","R542","R566","L62","R96","L1","L75","L99","R57","L62","L936","R16","R34","R10","R50","R6","L27","L9","L60","L21","L22","L61","R988","L20","L19","R85","L52","L82","L46","L37","L17","L75","R775","R80","L80","L42","R34","L92","R897","R74","L83","L88","L922","L278","R67","R33","L94","R94","L10","R10","L523","R47","R76","L193","R491","R16","L14","R379","R26","L5","L823","L15","R21","L57","L26","R446","L959","R13","R18","R29","L47","R496","L96","R90","L90","L607","R79","L37","L96","L39","R38","L38","L15","R15","L93","R5","L12","R60","L59","L336","L65","L954","L46","R58","R18","R12","R12","R83","L37","L92","L94","L60","L41","L55","L37","L21","R77","R35","L53","R94","L72","R73","L25","R89","R92","L87","L90","L12","L81","L70","L56","L60","R88","R92","R20","R69","R31","R8","R92","L235","R335","R139","R91","L99","L78","R20","L87","R137","L19","L4","L58","L97","R982","R973","L96","R95","R1","L94","R8","R63","R385","R36","L47","L555","R41","L37","R7","L72","R723","L58","L106","L94","R46","R54","R71","L194","L75","R98","L48","L14","R83","L594","R73","L8","L36","L20","R46","R918","L59","R659","R28","R24","R65","R24","L17","L64","L60","R48","L19","L106","R77","R28","R703","R69","L7","R7","L68","R268","R89","L250","L39","R59","R30","R1","L504","L31","R45","L76","L124","R78","L803","R265","R46","L30","L45","R94","R595","R44","L6","L84","R6","L60","R77","L589","R827","L37","L31","L47","R20","R72","R808","L33","L62","L705","L35","L65","R65","R61","R5","R38","R31","R718","L18","R19","R81","L16","L64","L38","L5","R82","L48","L15","R73","L25","R632","L388","R56","R395","L588","L38","L87","L97","L29","R60","R12","L22","R25","R25","R58","R123","L39","L198","L441","L803","R64","L64","L72","R728","R67","L823","R15","L12","L76","R73","L39","L54","L7","L22","L78","L43","R96","L87","L78","L21","L67","L60","R36","R2","R96","L7","L29","R434","R81","L415","R73","R46","L83","R894","R64","L32","L93","R67","L74","R48","L45","L3","R390","R69","L39","L34","L45","R79","R80","L26","L93","L63","L18","R58","L58","L6","R54","L6","R58","L64","R69","R41","R54","R6","L22","R504","R81","L97","R1","R27","L88","R88","R21","L21","L84","R897","L73","L54","L987","L57","L40","L251","L51","L30","R47","L53","L71","R7","R90","R20","R90","L191","R124","R98","L672","L59","L27","L73","L47","L48","R95","R1","L1","R55","R545","L99","L93","L2","R94","R78","R22","L49","L63","L167","R80","L56","L45","R65","R574","L64","R68","R771","L34","R38","R12","L91","L29","R390","R91","L37","L54","R95","R5","L25","L275","R34","L34","L28","R628","R675","R247","R57","L5","L74","R32","R68","R56","R49","L58","L47","R55","R58","L13","L40","L199","R39","L44","R71","L6","L21","R37","L31","L6","L9","R69","R20","R47","L27","L42","L58","L86","L5","R758","L18","L67","R718","R678","L23","L8","R35","R18","R15","R18","L56","R864","L41","R91","L91","L187","L81","L95","R7","L58","L374","R57","L67","L29","R27","L980","R67","R906","L93","L423","L49","R45","R36","L9","L7","L57","R20","L56","R42","L8","R99","R309","R39","L95","L187","L381","R45","L15","L988","R40","L51","L105","L44","R25","L47","L16","L56","L206","R70","R821","R76","R33","R86","L50","R136","L72","L45","R4","R56","L58","R643","L90","L10","R689","R96","R74","L26","R67","L241","R896","R93","R52","L46","R446","R41","R823","L26","L38","R33","L3","L930","R555","R53","R830","R4","L442","L570","R32","R38","L41","R7","L60","R522","L28","R14","L36","R5","R18","L58","R686","R5","L28","L6","L79","L16","R95","R93","L231","L62","R16","L216","R986","R90","L76","L53","L47","L692","R557","L60","L3","R98","L889","R1","R88","L64","R34","L970","L304","R4","L10","R910","R28","L89","R61","L46","L38","L18","L28","R30","L56","R56","L58","R958","R143","R1","R56","L43","R7","R36","L10","L51","R21","R34","L310","R16","L16","R16","L152","R86","L81","R47","L63","L337","R67","R13","L680","R52","L732","L74","L89","L517","R27","R83","L50","R12","R817","L80","L67","L82","R26","L98","L28","L78","L6","R84","R42","L55","L75","L59","L42","L67","L21","R547","L25","R83","L28","L40","L60","R101","L999","L240","L62","R85","L11","R26","R3","R347","L87","L63","L52","R16","L64","L89","R75","L99","R51","L38","L12","L24","R2","R79","L41","L261","L18","L83","L42","R2","R44","L46","R70","L70","R50","L150","L442","R42","L85","R585","R59","L466","R82","R25","R708","L8","R56","R6","R39","L11","L937","R64","L28","L729","L60","L48","R48","L73","L82","R68","R65","L13","R535","L85","R12","R16","L42","R16","R83","L86","L56","R64","R78","R32","R4","L91","R93","R102","L86","R86","R58","L98","R4","L822","L82","L1","R28","L92","L22","R28","R46","L37","L16","L78","R360","R84","L27","L11","L62","R17","L25","L92","R55","R52","L63","R22","R34","R9","L9","L59","R36","L77","R20","R80","R13","L7","L99","L67","L40","L4","R99","L52","R59","R86","R74","R38","L6","L94","R29","L29","R60","R69","L39","L45","L97","L41","R68","L31","L26","R12","R66","R4","R26","R74","L18","L56","L2","L24","L32","L28","L2","L50","R50","L28","L9","R23","R8","R4","L17","L6","L44","R46","R4","R3","R18","L37","R42","L7","L21","L41","R18","L1","R42","R50","L20","R24","L38","L47","L26","R25","R6","R3","L33","L3","R7","L19","L7","L2","R31","R43","R21","R12","R47","R45","L31","L40","R44","R24","L34",\;</v>
+        <f>_xlfn.CONCAT("const listOfInputs = ",CHAR(91),D1:D4104,CHAR(93),";")</f>
+        <v>const listOfInputs = ["R9","R19","R34","R38","L47","R30","R36","L35","L25","L10","L6","R38","R16","R43","L37","R48","R23","L19","R22","L17","R1","R13","R26","R11","R31","R42","L22","R41","R21","R3","R24","L22","L28","L6","L21","L37","L17","L25","R43","L21","L4","L28","R16","L49","R46","R37","R14","R42","L12","L29","L36","L64","R67","L12","L96","L93","R38","R96","R70","L43","L27","R29","R43","L95","L72","L5","L73","R73","L3","R83","L88","L69","R86","R20","L97","R70","L77","R75","R40","L95","L10","R50","L85","R84","R16","R74","L74","R43","L85","L58","L95","R95","L44","R44","L68","L32","L97","L4","R50","R32","R19","L29","R829","R41","L15","L26","L83","L77","R60","L74","R34","L91","L22","R53","R898","L98","R49","R51","R99","R70","L69","L24","R24","R5","R95","L48","L38","R66","R61","R33","L74","R762","L750","R90","L802","L10","R190","L80","L85","L15","R738","L54","R16","R81","L90","R38","R76","R65","L76","R71","R35","L85","L54","L261","R868","L3","R663","R72","R22","R37","L59","R524","L12","L12","R69","L47","R974","R579","R84","R276","L35","R350","L50","L36","R36","R7","R11","R89","R87","R6","R23","R93","L16","L43","R33","R635","L16","L86","R52","L575","R74","R26","R10","R96","L6","R33","L505","R84","R98","L59","L831","L39","R21","L2","L606","L45","L90","L63","R47","R80","R985","R29","L237","R41","L3","L38","L44","R27","L83","L89","L65","R27","L86","R89","L32","R44","R212","L74","R97","R77","R91","R9","R83","R17","L55","R9","R46","R480","L63","R83","L71","L29","R252","L567","L97","R56","R56","L77","R22","R86","R8","L23","R84","R91","L44","R23","L70","L21","R21","R27","R12","R24","R37","L206","R360","L241","L12","L93","L48","L96","L95","L18","R23","L14","R46","R69","R25","R7","L68","L44","R5","L268","R68","R1","L1","R280","L980","L131","L192","R34","R36","L47","L37","L145","L948","R930","R14","R46","R40","L517","L24","L836","R37","L960","L49","L31","R535","L55","L11","R72","R56","R83","R25","L225","L70","L25","L48","L966","R709","L9","L91","R53","L5","R52","L14","R641","R73","L57","R960","R36","R26","R477","L85","R609","L66","L28","R54","L26","L41","L69","L6","L49","R18","L19","R45","R21","R44","L32","R88","L65","R6","R45","L75","R24","R133","R32","R81","L6","R29","L504","R77","L84","R58","L39","R57","L969","L55","L5","L864","R81","L43","L14","R10","L128","L85","R3","R9","L9","R99","R207","L84","L90","R71","R278","R58","L39","L33","L67","L378","R58","R92","L6","R34","L89","L55","R94","L78","L77","R55","R650","L4","R67","L191","L772","L72","R84","R59","L97","R26","R98","R48","R16","R19","R13","L44","R50","R71","R29","R27","L14","R687","R79","R236","L396","R81","L27","L32","R659","L54","R67","L13","L92","R6","L17","R10","R426","R793","L14","L35","R28","L5","R53","L23","L21","L31","R822","L35","L579","R30","R37","R50","R194","R3","R53","L940","R309","R378","L91","R7","L52","R65","L26","R16","R237","R68","L581","L26","R83","L92","L45","R176","R49","L45","R18","R481","R68","R44","L63","L291","R67","L554","L721","L7","R15","L53","R53","R69","R14","R94","R35","R12","L24","L90","L36","L66","L939","R31","L70","R970","R562","R85","L23","R95","R81","L19","L33","L48","R53","L129","R76","R216","L91","R95","L20","R69","L65","R96","R72","R28","R17","L11","L96","R170","L87","R33","L83","R657","R65","R58","R72","R5","R49","L38","L34","L477","R87","L69","L75","L913","R995","L25","R66","L19","R258","L537","R13","R19","R53","L53","R74","L74","R938","R95","L33","R72","R28","L64","R25","L56","L272","R73","R68","L41","R22","R6","L961","L825","R325","R67","R95","R38","R41","L68","R27","L75","R75","L97","R60","L62","R90","L73","L393","R25","L50","L375","L67","L58","L92","L608","R13","L295","L18","R63","L95","R32","L952","L18","R799","L80","L48","L1","R10","R90","L824","R91","L67","L24","R33","R16","L25","R76","R24","R63","L40","R1","R66","L90","L74","R374","L87","R942","R945","L83","R64","L89","R32","L577","R9","R13","L59","L87","L21","L356","L46","R421","R79","R55","L42","R87","L53","L47","L66","L49","R15","R81","R73","R822","R923","L454","R44","L89","R23","L592","R69","L18","R17","R65","L89","R55","L30","R61","R53","R82","R97","R605","R2","L3","R814","R1","R64","L76","R39","R21","R40","R105","R23","R72","R54","R533","R28","L15","L49","R49","L92","L2","L206","L69","R82","L913","L89","L11","L25","L151","R76","L43","R97","L54","R859","L274","L322","L134","L29","L83","R583","L685","R366","L7","L10","R36","R33","R35","L43","R82","L7","R593","R492","L85","L927","R4","L53","L24","R29","R222","L922","L594","R41","L76","R251","L47","L57","L91","L56","R24","L22","L70","R31","R525","L32","L796","R56","R7","R677","R29","R88","R65","R18","R19","L23","R904","L23","R41","L318","R65","R42","L99","L63","R15","L78","L57","L33","L84","R34","R87","R624","L30","L97","R24","R35","R67","R48","L59","L35","L70","L97","L69","L55","L550","L82","L89","R78","R828","L44","R286","R558","R42","L13","R53","R58","R63","R808","R999","L457","R47","R94","R65","L88","R30","L48","L75","R523","R32","R70","L3","R93","R59","L52","R51","R2","R897","L914","L36","L47","L861","R65","R91","R38","R32","R282","R10","R16","R70","L16","L38","R58","L21","R81","L78","R18","L422","R22","L304","L96","L54","R61","R32","L39","R371","L71","L89","L8","L403","L688","L21","L388","R16","R807","R82","R161","R96","R635","R426","R38","L59","R58","L17","R619","L59","L93","L13","L384","L16","L5","L636","L68","L91","R66","L66","R31","L63","L57","L56","L55","R853","R464","L92","R475","L640","R40","L16","L484","R87","R87","L394","L80","R64","L42","R12","L39","L31","L25","L49","R48","R62","L90","R90","L78","R13","R89","R74","R77","L549","L4","L22","R89","R54","L8","L35","L61","R27","R41","R7","R86","L27","L73","L42","R88","R818","L15","R58","L48","L5","R780","L24","L1","L9","L3","L97","R64","L9","R16","L71","R893","L87","R427","R55","R5","L93","L36","R1","L89","L60","R91","L7","R83","L51","L55","R23","L7","R7","L65","R65","R1","L24","L35","R658","L51","L149","R88","R1","L89","R74","L74","L644","R218","L52","R78","R21","L21","L296","R96","R909","L38","R343","L45","L62","L702","R77","L682","L21","R21","R72","R428","L61","L39","R61","R39","R94","L51","R22","R725","R482","R28","L84","R84","L56","R56","R502","R24","L364","L865","R403","R25","R575","L74","L89","R863","R51","L220","L31","R8","L73","L35","L29","R199","R96","R72","L76","L60","R67","L43","R74","R955","R79","R17","L12","L2","L20","R29","R95","L46","R589","R16","R11","L151","R76","L36","R737","R63","R19","L69","R50","L53","R242","L47","L96","R69","L15","L72","R65","R939","L92","L56","L84","R76","R24","R92","L59","L454","R36","R82","L97","R66","L394","R14","L76","R20","R28","R47","L5","L581","L19","R67","R11","R46","R69","L93","L1","L4","L95","L50","R85","R382","L98","L8","R9","L20","R92","R8","R2","L6","R704","R98","L86","R60","R99","R66","R63","L867","L333","R21","R67","L74","L14","R7","L12","R52","L17","L130","L659","R505","R79","R75","L69","L81","R50","L6","L40","R46","L72","R57","R41","R74","R25","R510","L35","R18","L436","L713","L91","L4","L374","L5","L95","R12","R88","L92","L19","R9","L98","R98","R984","R18","R68","R32","R61","L26","L76","R36","L65","R70","L339","R39","L89","R30","R30","L115","L56","R705","L18","L936","R64","R85","L74","L795","L31","R57","R46","L425","R92","L70","R71","L98","R727","R12","R479","R109","R1","L4","R60","R43","R815","R316","L440","R11","L55","L88","R97","L70","L38","R50","R2","R24","R76","L19","L81","R537","R63","L16","L35","R690","L2","L6","L31","R44","L49","R905","R44","R32","L473","L8","R39","R67","R78","L18","R334","L92","R97","L8","L13","R18","L97","R226","R74","R94","R179","R67","R860","L247","L72","R21","R98","R59","R9","L78","L525","L65","R89","L16","R27","R55","L198","L53","R96","R31","L731","L29","R29","L9","R35","R62","R530","R404","R78","R15","L815","L799","L201","L92","R98","L506","R31","L27","R302","L50","L69","L34","R97","L363","L58","R97","L59","R91","R42","L16","R16","R839","R61","L828","R26","L49","L49","R87","R813","L63","R891","R372","L94","R253","R39","L367","R869","L73","L33","R72","L166","L201","R96","R38","R58","L91","L45","L36","L719","R12","L89","L38","R15","R313","L77","L36","L41","R48","R50","R543","R78","R98","L12","R24","L665","R4","L27","R30","R414","R6","L12","R97","R22","L870","R62","L49","L26","L31","L43","L66","R231","L19","R46","R30","L22","R13","R57","L151","L819","L88","R64","L76","R40","L840","R59","L64","L46","L81","L926","R579","L68","L270","L83","L55","R55","R774","L74","R92","L5","R75","R54","R84","R77","L277","L703","L97","L3","R96","L93","R29","R3","R60","L32","L68","L592","R98","R2","R6","L871","L22","L53","L49","L611","L89","L32","R47","L319","L42","L65","R68","L68","L21","R21","L695","L5","L770","R95","R75","R6","L85","R79","L28","L72","R98","R48","R945","L15","L52","L44","L32","R980","R72","L6","L408","L79","R693","L32","L13","L12","L18","R94","R81","R162","R638","R738","L38","R91","L29","R46","R167","L9","L355","L96","L27","L59","L29","R23","R77","L36","R57","L21","L69","L31","L940","L960","L36","R67","R35","R29","R5","R24","R78","R98","L26","R69","L47","R4","L41","R41","L83","L74","R80","R21","R56","R684","R51","L35","R863","L23","R61","L801","L47","R51","R80","R81","L7","R442","R27","R73","R73","R87","L963","L97","R14","L14","L24","R15","L291","R33","R97","L263","R11","R12","R10","R445","L12","L45","R612","L519","L81","R53","L53","L65","R565","R34","R66","L93","R16","R58","R25","L81","L17","R92","R55","R56","R40","L15","R67","R97","R93","R7","L69","R59","L42","R24","R74","R654","R24","L24","R35","R65","R34","R81","L4","R8","L59","R53","R57","L70","L33","R90","R92","L49","R54","R51","L119","L11","L75","R56","L528","R572","L14","L86","L9","R9","L73","R84","L311","R86","L86","L60","L40","R45","R155","L74","R93","R595","R83","L301","L90","L52","L1","L74","R99","R297","R32","L753","R46","R29","R299","L306","L22","L75","R62","L87","R88","L14","L246","R21","L14","L55","L80","R86","L33","L53","R508","R592","L6","L15","R6","L47","L95","R29","L72","L332","R432","L446","L58","L96","L40","R66","R17","R457","R57","R75","L950","R32","R95","L9","L55","R206","R23","L96","L78","R27","L115","L12","R3","R18","R79","L33","L62","R53","L6","L52","R60","R40","L27","R97","R27","R3","R495","R207","L2","L10","R73","L63","R94","L39","R92","L75","R28","R82","R18","R978","R22","L8","L92","L61","L909","R102","L32","R40","R19","L40","L419","L7","R7","L25","R25","R53","R247","L37","L763","L56","R604","R296","R56","R40","R94","R694","L13","L88","R203","L66","R33","L41","R44","L679","L531","L2","R3","R22","L74","L47","L31","R54","R85","L564","L930","L642","L81","L69","L79","L20","R485","L503","L42","R293","L93","L55","R13","L13","L8","R896","L34","R272","L26","R73","L762","L11","R90","R510","L313","R51","R228","L66","L23","R28","R94","L899","R38","L38","L77","L589","L50","R16","L88","R42","L82","L72","L28","R528","R47","L93","L54","R14","L14","L49","L51","L50","L63","R54","L41","L86","R43","R81","R88","L79","L47","L24","L76","R93","R891","R21","R95","L56","L37","R689","R53","R51","R26","R161","R30","R83","R82","R98","R17","R98","R805","R68","L92","L4","R28","L418","R95","R53","L33","L497","L13","L282","R43","L69","L59","R80","L37","L55","L32","L40","L87","R421","R67","R963","L77","R77","L323","R147","R239","R7","R30","L35","R985","R50","R10","L921","L89","R23","L188","L73","R10","L72","L83","R18","L7","R72","R5","L5","L56","R51","L20","L75","L43","R26","L82","R83","L872","L551","R7","L68","L94","R44","R56","R4","L10","R82","R30","L44","L603","R685","L98","L70","R9","L47","R36","R587","R80","R55","L302","L96","L47","R54","L11","L92","L8","L61","R61","R71","R58","L29","L24","L6","L22","R98","R660","R94","L15","R515","L211","R11","R42","R45","R813","L66","L50","R30","L114","R60","R57","L96","L21","L641","L59","L49","R425","L76","R18","R82","L69","L26","L980","L40","L85","R75","L90","R15","R50","L55","L95","R891","L891","R311","R741","R9","R639","L581","R81","R29","R71","L12","L94","R16","L10","L82","L70","R36","L84","R553","L53","L10","L90","R730","R32","R38","L26","R26","L418","R65","R47","R6","L40","L60","L7","R307","R84","R416","R26","R92","L22","R42","L62","L76","L380","L66","L54","L772","R72","R62","L33","R71","L12","L64","L24","L56","L95","L8","R59","R90","L90","L83","R38","L55","L889","L77","R466","R76","L790","L44","R58","R31","L71","R40","R74","L74","R5","L19","R214","R16","L16","R6","L65","R59","L56","R7","L357","L77","L47","R734","L15","L39","R66","R55","R371","R48","L684","L6","L71","L929","R82","L83","R1","L33","R61","L13","R30","L52","L93","L61","L39","R61","L61","L94","L509","R94","R95","R14","L45","L55","R72","L22","R650","L661","R61","L64","L36","L87","R887","L83","R12","R82","R646","R84","L57","L55","L97","R90","L32","L90","R476","R31","R93","R320","R80","R24","L78","L46","L90","R3","R22","R33","L31","L694","R22","R335","R86","R314","R66","L458","R92","R363","R50","L99","L13","R6","L7","R690","R706","R22","L99","R69","L88","R19","L3","L16","L377","L64","L57","L3","L90","R53","R38","L21","R44","R77","R3","L29","L74","R34","R98","L932","R10","R81","R760","R77","L927","R99","L42","R73","R95","R899","R75","L41","L17","R78","R70","L90","R53","L37","R25","L86","R13","L72","R61","R759","L14","L78","R24","R252","R17","L17","L89","L49","L62","R222","R21","L43","R2","R41","R49","R42","L81","R67","R4","L27","R60","L57","L305","L11","L84","L72","L352","R256","L838","R19","L51","L62","L35","L65","L92","L58","R689","R61","R201","R399","L63","R83","L97","R77","R575","L75","L73","L72","L395","R26","R629","L61","L35","L44","R825","L34","R34","L56","R68","R88","R92","R608","L260","R89","L829","R74","R17","L91","L26","L564","L10","L98","L802","R12","L12","R33","L933","L58","R67","R17","L26","R83","R92","R25","L399","L1","L16","R61","R108","R47","L621","L73","R24","L848","L71","L454","R543","L213","L40","L62","R15","L86","L77","L37","R37","L637","R63","L75","R12","R23","R77","R9","R23","L743","L89","R948","L902","R54","R66","L352","L17","R3","L43","L80","L78","R201","L4","L58","L438","R39","L25","L67","L55","L294","R7","L93","L212","L71","R71","R781","R27","L72","R11","R45","L97","R240","L13","L56","L66","L90","R7","L17","L21","L38","L41","L36","L37","R473","L31","L32","L637","R19","L19","L49","L65","L86","L838","L7","L859","R55","R28","R21","L138","R438","R30","L30","L51","R324","R96","L69","L31","R79","L48","L95","L5","R121","R79","L324","R17","L93","L534","L7","L937","R97","R983","R3","L84","L21","R4","R533","L437","L1","R47","R16","L12","L265","R2","R13","L71","R71","L99","R81","R18","R821","R57","R22","L67","R89","L49","L73","R77","R680","R79","R10","R83","L29","L87","R248","L10","L23","R79","L367","R23","L463","L86","R97","L91","R69","L64","L757","R3","R29","R21","L201","R80","L58","L42","L230","L52","L35","R39","L4","L177","L26","L55","R740","L96","L261","L83","L99","R57","L18","L52","L76","L372","R45","L35","L59","R34","R375","L277","L96","R916","R96","L55","L146","L171","L127","R42","L42","L507","R33","R74","L88","R58","L20","R50","R31","L11","L20","L26","R694","R39","L39","R58","L998","R36","R89","R21","R76","L80","R32","L76","R80","L6","R54","L20","R56","L290","L90","L10","R21","L29","R8","L97","R23","R73","R23","L22","L54","L9","L55","R334","R91","L20","R113","R467","R833","L93","R544","R78","R61","L90","L75","L25","R695","L95","L70","R470","L92","L11","L97","L38","L11","R51","L91","L82","L29","R30","L844","L86","L22","R722","R99","R446","R55","L8","R525","R83","L13","R72","L92","R333","L33","L67","R439","R461","L790","L566","L97","R53","L66","R14","L9","L39","L60","R68","R91","L38","L61","L890","L910","R774","R826","L97","L33","L56","L5","L39","R930","L295","L59","R54","R3","R797","R71","R61","R28","R53","R26","R96","R82","L126","R66","R43","R70","R20","L421","L71","R70","L19","L52","L597","L97","R97","L85","L15","L70","R76","R94","R79","R13","L92","R51","R58","R49","R63","R16","R48","R15","L38","R26","R12","R62","L62","L24","R81","R43","R1","R899","R58","L753","L56","R18","R26","R1","R6","R33","R67","L58","L72","L770","R41","R46","R87","L437","L34","R63","R34","L60","L73","L2","L88","R23","L11","L75","L414","L84","R84","L40","L87","R327","L90","R53","L92","L71","L875","L44","L50","L5","R94","R32","L96","R13","L69","R28","L28","L58","R92","R94","R63","L568","L423","L22","R4","R67","L29","R69","R11","R7","L7","L5","L227","R32","L26","L74","L7","L921","L487","R15","R927","L95","R62","L93","R2","L3","R50","L50","L99","R99","L691","L134","L75","L76","R670","R53","L491","L352","L10","R6","R19","L79","R23","L837","R55","L23","L46","L12","L22","L76","L31","L286","R50","R65","L28","L54","R82","R88","R699","L158","L22","L89","R98","L199","R461","R22","R1","R899","L126","L74","L55","R555","R1","L31","R78","L39","R846","R45","R20","L71","R78","R27","R21","R925","R36","R71","R68","L375","L66","R489","L523","R29","L29","R6","L306","L889","L11","L73","L95","L307","R7","L11","L51","R630","L82","L5","L638","R25","R688","R4","R8","L89","L95","L21","R57","R48","R29","R914","L96","R53","L561","L39","R14","L14","R35","L351","R38","R576","L34","L964","L76","R176","L88","R83","R436","R471","R96","R7","R56","L95","R5","R82","R41","L57","L37","R476","L76","R46","L90","L93","R7","R81","R570","R79","L68","L86","R92","R32","R30","L648","L52","R65","R237","L94","R39","L947","L2","L998","R23","R64","L195","L92","R663","R66","R72","L97","L807","L978","R81","R21","L68","L895","R16","L1","L54","R99","L6","R77","R59","L83","R35","R45","L45","R4","L28","L4","R28","L753","R377","R76","L98","L931","L43","R28","R477","L33","L22","L378","L74","R74","R947","L505","L58","R16","L74","L982","L866","L37","R59","L774","R636","L3","R41","R523","L23","L84","L437","L79","L71","R71","L22","L74","L76","R72","R93","R7","R89","L89","R7","R11","R724","R68","R190","L54","L827","R245","L64","L79","L17","R938","R83","L35","R10","R52","R943","R73","R6","L68","L6","L56","L544","L39","L849","L867","R55","L715","L70","L48","L67","R96","R79","R25","R639","L39","L60","R55","L95","L88","L12","R62","R272","R85","R81","R67","L78","L56","L58","L201","R80","R46","R97","L95","R98","L1","R815","L14","L57","L95","R52","L22","R22","R19","R34","L78","R25","L20","L863","L17","L93","L97","R77","L44","R84","R17","R56","R1","R199","L91","L864","L188","R43","R95","R726","L73","R44","R8","L65","R65","R29","R786","L85","R70","L72","R577","R495","R96","R4","L51","R39","R12","L13","L42","L87","R46","L4","R63","R29","L57","L411","L745","L60","L1","L518","L75","L25","L910","L28","L62","L67","L65","L68","R19","R81","R74","L74","R41","L72","L769","L68","R68","L35","R35","R92","R88","R20","R76","L76","R78","L478","R28","R72","R69","L69","L10","R10","R806","R13","R81","L31","R57","L16","R289","L23","L62","L40","L74","L77","L28","R5","R544","R47","L57","L88","R47","R311","R9","L13","R55","L38","L17","L22","R22","L50","R750","R175","L93","L82","R9","R98","R73","L2","R22","L34","L37","R59","L88","R361","L1","R4","R36","L29","L42","R40","L93","L76","L82","L36","L17","L420","L50","R71","L94","L720","L441","R89","L726","R826","L741","L59","L46","L213","R464","R95","R98","L98","R135","L23","R21","R67","R56","L56","R54","R46","R33","L33","R45","R55","L635","R306","L2","R74","L678","R26","L99","R18","L10","L71","L29","R83","R213","L478","R19","R63","R796","L71","R59","R19","R48","L15","L17","L18","R26","L27","R9","R163","L507","R41","L6","R25","R579","L4","R949","R43","R8","R68","R22","R51","R35","R38","R388","R66","L68","R71","L71","R54","L54","R477","R14","R75","R32","R650","R30","L78","R34","L34","L65","L99","R44","L80","R339","L78","L23","L87","R37","R86","L474","R27","L94","L33","L75","L25","L57","R57","R26","R75","R352","R5","R42","L49","L69","R196","R61","R26","R43","R9","R14","L37","R11","L105","R41","R37","R8","L86","L85","L15","L154","L746","L571","R30","L59","L2","R11","L84","R66","R41","L32","R44","R56","R35","L26","R15","L43","L81","R32","R68","R22","R78","L976","R76","L776","L21","L3","R980","R76","L656","L42","L858","L288","R188","R15","R39","R67","R72","R98","L970","L28","L793","L56","R240","L86","R40","L77","L14","R14","R41","R95","L1","R4","L270","R70","L10","R48","R62","L99","L1","R626","L26","L33","R231","L63","R65","L47","R91","R6","L92","R542","R566","L62","R96","L1","L75","L99","R57","L62","L936","R16","R34","R10","R50","R6","L27","L9","L60","L21","L22","L61","R988","L20","L19","R85","L52","L82","L46","L37","L17","L75","R775","R80","L80","L42","R34","L92","R897","R74","L83","L88","L922","L278","R67","R33","L94","R94","L10","R10","L523","R47","R76","L193","R491","R16","L14","R379","R26","L5","L823","L15","R21","L57","L26","R446","L959","R13","R18","R29","L47","R496","L96","R90","L90","L607","R79","L37","L96","L39","R38","L38","L15","R15","L93","R5","L12","R60","L59","L336","L65","L954","L46","R58","R18","R12","R12","R83","L37","L92","L94","L60","L41","L55","L37","L21","R77","R35","L53","R94","L72","R73","L25","R89","R92","L87","L90","L12","L81","L70","L56","L60","R88","R92","R20","R69","R31","R8","R92","L235","R335","R139","R91","L99","L78","R20","L87","R137","L19","L4","L58","L97","R982","R973","L96","R95","R1","L94","R8","R63","R385","R36","L47","L555","R41","L37","R7","L72","R723","L58","L106","L94","R46","R54","R71","L194","L75","R98","L48","L14","R83","L594","R73","L8","L36","L20","R46","R918","L59","R659","R28","R24","R65","R24","L17","L64","L60","R48","L19","L106","R77","R28","R703","R69","L7","R7","L68","R268","R89","L250","L39","R59","R30","R1","L504","L31","R45","L76","L124","R78","L803","R265","R46","L30","L45","R94","R595","R44","L6","L84","R6","L60","R77","L589","R827","L37","L31","L47","R20","R72","R808","L33","L62","L705","L35","L65","R65","R61","R5","R38","R31","R718","L18","R19","R81","L16","L64","L38","L5","R82","L48","L15","R73","L25","R632","L388","R56","R395","L588","L38","L87","L97","L29","R60","R12","L22","R25","R25","R58","R123","L39","L198","L441","L803","R64","L64","L72","R728","R67","L823","R15","L12","L76","R73","L39","L54","L7","L22","L78","L43","R96","L87","L78","L21","L67","L60","R36","R2","R96","L7","L29","R434","R81","L415","R73","R46","L83","R894","R64","L32","L93","R67","L74","R48","L45","L3","R390","R69","L39","L34","L45","R79","R80","L26","L93","L63","L18","R58","L58","L6","R54","L6","R58","L64","R69","R41","R54","R6","L22","R504","R81","L97","R1","R27","L88","R88","R21","L21","L84","R897","L73","L54","L987","L57","L40","L251","L51","L30","R47","L53","L71","R7","R90","R20","R90","L191","R124","R98","L672","L59","L27","L73","L47","L48","R95","R1","L1","R55","R545","L99","L93","L2","R94","R78","R22","L49","L63","L167","R80","L56","L45","R65","R574","L64","R68","R771","L34","R38","R12","L91","L29","R390","R91","L37","L54","R95","R5","L25","L275","R34","L34","L28","R628","R675","R247","R57","L5","L74","R32","R68","R56","R49","L58","L47","R55","R58","L13","L40","L199","R39","L44","R71","L6","L21","R37","L31","L6","L9","R69","R20","R47","L27","L42","L58","L86","L5","R758","L18","L67","R718","R678","L23","L8","R35","R18","R15","R18","L56","R864","L41","R91","L91","L187","L81","L95","R7","L58","L374","R57","L67","L29","R27","L980","R67","R906","L93","L423","L49","R45","R36","L9","L7","L57","R20","L56","R42","L8","R99","R309","R39","L95","L187","L381","R45","L15","L988","R40","L51","L105","L44","R25","L47","L16","L56","L206","R70","R821","R76","R33","R86","L50","R136","L72","L45","R4","R56","L58","R643","L90","L10","R689","R96","R74","L26","R67","L241","R896","R93","R52","L46","R446","R41","R823","L26","L38","R33","L3","L930","R555","R53","R830","R4","L442","L570","R32","R38","L41","R7","L60","R522","L28","R14","L36","R5","R18","L58","R686","R5","L28","L6","L79","L16","R95","R93","L231","L62","R16","L216","R986","R90","L76","L53","L47","L692","R557","L60","L3","R98","L889","R1","R88","L64","R34","L970","L304","R4","L10","R910","R28","L89","R61","L46","L38","L18","L28","R30","L56","R56","L58","R958","R143","R1","R56","L43","R7","R36","L10","L51","R21","R34","L310","R16","L16","R16","L152","R86","L81","R47","L63","L337","R67","R13","L680","R52","L732","L74","L89","L517","R27","R83","L50","R12","R817","L80","L67","L82","R26","L98","L28","L78","L6","R84","R42","L55","L75","L59","L42","L67","L21","R547","L25","R83","L28","L40","L60","R101","L999","L240","L62","R85","L11","R26","R3","R347","L87","L63","L52","R16","L64","L89","R75","L99","R51","L38","L12","L24","R2","R79","L41","L261","L18","L83","L42","R2","R44","L46","R70","L70","R50","L150","L442","R42","L85","R585","R59","L466","R82","R25","R708","L8","R56","R6","R39","L11","L937","R64","L28","L729","L60","L48","R48","L73","L82","R68","R65","L13","R535","L85","R12","R16","L42","R16","R83","L86","L56","R64","R78","R32","R4","L91","R93","R102","L86","R86","R58","L98","R4","L822","L82","L1","R28","L92","L22","R28","R46","L37","L16","L78","R360","R84","L27","L11","L62","R17","L25","L92","R55","R52","L63","R22","R34","R9","L9","L59","R36","L77","R20","R80","R13","L7","L99","L67","L40","L4","R99","L52","R59","R86","R74","R38","L6","L94","R29","L29","R60","R69","L39","L45","L97","L41","R68","L31","L26","R12","R66","R4","R26","R74","L18","L56","L2","L24","L32","L28","L2","L50","R50","L28","L9","R23","R8","R4","L17","L6","L44","R46","R4","R3","R18","L37","R42","L7","L21","L41","R18","L1","R42","R50","L20","R24","L38","L47","L26","R25","R6","R3","L33","L3","R7","L19","L7","L2","R31","R43","R21","R12","R47","R45","L31","L40","R44","R24","L34",];</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.25">
@@ -39929,5 +39929,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>